<commit_message>
nova data zeny 4x
</commit_message>
<xml_diff>
--- a/data/women/W_2021_09_MCR.xlsx
+++ b/data/women/W_2021_09_MCR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\data\women\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE726DC5-E7D7-40C1-8CAC-60BBD169824B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379E890A-EBF8-4D8C-83C6-75A6A8CB2169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9444" yWindow="228" windowWidth="13128" windowHeight="12180" tabRatio="707" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11304" yWindow="-15588" windowWidth="14928" windowHeight="15444" tabRatio="707" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initiation" sheetId="1" r:id="rId1"/>
@@ -724,7 +724,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C15"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1483,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADB98C0-9A13-4D8D-A7A8-55BD7C982938}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1581,10 +1581,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1622,10 +1622,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -2688,10 +2688,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D30" t="s">
         <v>6</v>
@@ -2729,10 +2729,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
@@ -3012,7 +3012,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{CADB98C0-9A13-4D8D-A7A8-55BD7C982938}"/>
+  <autoFilter ref="A1:M1" xr:uid="{CADB98C0-9A13-4D8D-A7A8-55BD7C982938}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M37">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3023,7 +3027,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="F6:G6"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4007,8 +4011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156E6CDF-EFAE-4C9F-ADCB-7E1D10DB3DAE}">
   <dimension ref="A1:K182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10371,7 +10375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F7FF14-8601-48E5-93A7-E4B2161D4AAD}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>